<commit_message>
Adjusted cash position exposure.
</commit_message>
<xml_diff>
--- a/etc/doc/Cryptotrader.xlsx
+++ b/etc/doc/Cryptotrader.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -4266,7 +4266,7 @@
         <v>1230</v>
       </c>
       <c r="D3" s="98">
-        <f t="shared" ref="C3:D18" si="0">D4-D$13/10</f>
+        <f t="shared" ref="D3:D11" si="0">D4-D$13/10</f>
         <v>0</v>
       </c>
       <c r="E3" s="73">
@@ -4281,16 +4281,18 @@
         <v>0</v>
       </c>
       <c r="H3" s="80">
-        <f>MAX(F3-MAX(G3-F3,0)/2,0)</f>
+        <f>MAX(F3-MAX(G3-F3,0)/$B$4,0)</f>
         <v>123</v>
       </c>
       <c r="I3" s="81">
-        <f>MAX(G3-MAX(F3-G3,0)/2,0)</f>
+        <f>MAX(G3-MAX(F3-G3,0)/$B$4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B4" s="71"/>
+      <c r="B4" s="71">
+        <v>10</v>
+      </c>
       <c r="C4" s="84">
         <f>C3-C$3/10</f>
         <v>1107</v>
@@ -4312,12 +4314,12 @@
         <v>12.3</v>
       </c>
       <c r="H4" s="84">
-        <f t="shared" ref="H4:H13" si="3">MAX(F4-MAX(G4-F4,0)/2,0)</f>
+        <f t="shared" ref="H4:H13" si="3">MAX(F4-MAX(G4-F4,0)/$B$4,0)</f>
         <v>110.7</v>
       </c>
       <c r="I4" s="85">
-        <f t="shared" ref="I4:I13" si="4">MAX(G4-MAX(F4-G4,0)/2,0)</f>
-        <v>0</v>
+        <f t="shared" ref="I4:I13" si="4">MAX(G4-MAX(F4-G4,0)/$B$4,0)</f>
+        <v>2.4600000000000009</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.15">
@@ -4348,7 +4350,7 @@
       </c>
       <c r="I5" s="85">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>17.22</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.15">
@@ -4379,7 +4381,7 @@
       </c>
       <c r="I6" s="85">
         <f t="shared" si="4"/>
-        <v>12.299999999999994</v>
+        <v>31.979999999999997</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.15">
@@ -4409,8 +4411,8 @@
         <v>73.8</v>
       </c>
       <c r="I7" s="85">
-        <f>MAX(G7-MAX(F7-G7,0)/2,0)</f>
-        <v>36.900000000000006</v>
+        <f t="shared" si="4"/>
+        <v>46.74</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.15">
@@ -4468,7 +4470,7 @@
       </c>
       <c r="H9" s="84">
         <f t="shared" si="3"/>
-        <v>36.900000000000006</v>
+        <v>46.74</v>
       </c>
       <c r="I9" s="85">
         <f t="shared" si="4"/>
@@ -4499,7 +4501,7 @@
       </c>
       <c r="H10" s="84">
         <f t="shared" si="3"/>
-        <v>12.299999999999994</v>
+        <v>31.979999999999997</v>
       </c>
       <c r="I10" s="85">
         <f t="shared" si="4"/>
@@ -4530,7 +4532,7 @@
       </c>
       <c r="H11" s="84">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>17.22</v>
       </c>
       <c r="I11" s="85">
         <f t="shared" si="4"/>
@@ -4561,7 +4563,7 @@
       </c>
       <c r="H12" s="84">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.4600000000000009</v>
       </c>
       <c r="I12" s="85">
         <f t="shared" si="4"/>
@@ -4604,7 +4606,7 @@
         <v>38</v>
       </c>
       <c r="C14" s="94">
-        <f t="shared" ref="C14:C23" si="7">C15-C$24/10</f>
+        <f t="shared" ref="C14:C22" si="7">C15-C$24/10</f>
         <v>0</v>
       </c>
       <c r="D14" s="102">
@@ -5257,7 +5259,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="94">
-        <f t="shared" ref="C35:C44" si="13">C36</f>
+        <f t="shared" ref="C35:C43" si="13">C36</f>
         <v>1230</v>
       </c>
       <c r="D35" s="102">

</xml_diff>

<commit_message>
Adjusted split price interval.
</commit_message>
<xml_diff>
--- a/etc/doc/Cryptotrader.xlsx
+++ b/etc/doc/Cryptotrader.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="440" windowWidth="25100" windowHeight="28360" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="26100" yWindow="440" windowWidth="25100" windowHeight="14180" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="MID" sheetId="3" r:id="rId1"/>
@@ -373,8 +373,8 @@
     <numFmt numFmtId="181" formatCode="#,##0_ "/>
     <numFmt numFmtId="182" formatCode="#,##0.0000000000_ "/>
     <numFmt numFmtId="183" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="186" formatCode="#,##0.000000_ ;[Red]\-#,##0.000000\ "/>
-    <numFmt numFmtId="187" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="184" formatCode="#,##0.000000_ ;[Red]\-#,##0.000000\ "/>
+    <numFmt numFmtId="185" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1662,46 +1662,46 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="183" fontId="2" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="186" fontId="3" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="184" fontId="3" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="3" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="2" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="4" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="2" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="4" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="2" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="2" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="3" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="3" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="3" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="185" fontId="3" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="185" fontId="3" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="185" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="185" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="119">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -1906,7 +1906,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2491,8 +2490,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="765005776"/>
-        <c:axId val="765008096"/>
+        <c:axId val="1383185280"/>
+        <c:axId val="1375941120"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2550,7 +2549,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2843,11 +2841,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="765012736"/>
-        <c:axId val="765010416"/>
+        <c:axId val="1257057360"/>
+        <c:axId val="1256994432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="765005776"/>
+        <c:axId val="1383185280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2904,12 +2902,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="765008096"/>
+        <c:crossAx val="1375941120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="765008096"/>
+        <c:axId val="1375941120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2965,12 +2963,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="765005776"/>
+        <c:crossAx val="1383185280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="765010416"/>
+        <c:axId val="1256994432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3012,12 +3010,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="765012736"/>
+        <c:crossAx val="1257057360"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="765012736"/>
+        <c:axId val="1257057360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3026,7 +3024,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="765010416"/>
+        <c:crossAx val="1256994432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11870,7 +11868,7 @@
   <sheetFormatPr baseColWidth="12" defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="171" customWidth="1"/>
-    <col min="2" max="8" width="10.7109375" style="171" customWidth="1"/>
+    <col min="2" max="8" width="12.7109375" style="171" customWidth="1"/>
     <col min="9" max="16384" width="12.85546875" style="171"/>
   </cols>
   <sheetData>
@@ -11904,7 +11902,7 @@
         <v>44</v>
       </c>
       <c r="C5" s="183">
-        <v>1.002</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.15">
@@ -11913,7 +11911,7 @@
       </c>
       <c r="C6" s="185">
         <f>C4*C5</f>
-        <v>1.503E-2</v>
+        <v>1.4985E-2</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.15">
@@ -11941,14 +11939,14 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B9" s="193">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="177">
-        <f>$C$5-$C$6*$B9</f>
-        <v>1.002</v>
+        <f>$C$5</f>
+        <v>0.999</v>
       </c>
       <c r="D9" s="178">
-        <f>C$9/C9-1</f>
+        <f t="shared" ref="D9:D28" si="0">C$9/C9-1</f>
         <v>0</v>
       </c>
       <c r="E9" s="189">
@@ -11956,11 +11954,11 @@
         <v>0</v>
       </c>
       <c r="F9" s="192">
-        <f>$C$5+$C$6*$B9</f>
-        <v>1.002</v>
+        <f>$C$5</f>
+        <v>0.999</v>
       </c>
       <c r="G9" s="178">
-        <f>F9/F$9-1</f>
+        <f t="shared" ref="G9:G28" si="1">F9/F$9-1</f>
         <v>0</v>
       </c>
       <c r="H9" s="189">
@@ -11971,571 +11969,571 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B10" s="194">
         <f>B9+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="181">
-        <f>$C$5-$C$6*$B10</f>
-        <v>0.98697000000000001</v>
+        <f>C9-$C$6*$B10</f>
+        <v>0.96902999999999995</v>
       </c>
       <c r="D10" s="182">
-        <f>C$9/C10-1</f>
-        <v>1.5228426395939021E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.0927835051546504E-2</v>
       </c>
       <c r="E10" s="199">
-        <f t="shared" ref="E10:E28" si="0">D10/$C$2</f>
-        <v>0.2538071065989837</v>
+        <f t="shared" ref="E10:E28" si="2">D10/$C$2</f>
+        <v>0.51546391752577514</v>
       </c>
       <c r="F10" s="197">
-        <f>F9+$C$6*$B10</f>
-        <v>1.0170300000000001</v>
+        <f t="shared" ref="F10:F28" si="3">F9+$C$6*$B10</f>
+        <v>1.0289699999999999</v>
       </c>
       <c r="G10" s="182">
-        <f>F10/F$9-1</f>
-        <v>1.5000000000000124E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.0000000000000027E-2</v>
       </c>
       <c r="H10" s="199">
-        <f t="shared" ref="H10:H28" si="1">G10/$C$2</f>
-        <v>0.25000000000000211</v>
+        <f t="shared" ref="H10:H28" si="4">G10/$C$2</f>
+        <v>0.50000000000000044</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B11" s="194">
-        <f t="shared" ref="B11:B28" si="2">B10+1</f>
-        <v>2</v>
+        <f t="shared" ref="B11:B28" si="5">B10+1</f>
+        <v>3</v>
       </c>
       <c r="C11" s="181">
-        <f>$C$5-$C$6*$B11</f>
-        <v>0.97194000000000003</v>
+        <f t="shared" ref="C11:C28" si="6">C10-$C$6*$B11</f>
+        <v>0.92407499999999998</v>
       </c>
       <c r="D11" s="182">
-        <f>C$9/C11-1</f>
-        <v>3.0927835051546282E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.1081081081081141E-2</v>
       </c>
       <c r="E11" s="199">
-        <f t="shared" si="0"/>
-        <v>0.51546391752577136</v>
+        <f t="shared" si="2"/>
+        <v>1.3513513513513524</v>
       </c>
       <c r="F11" s="197">
-        <f>F10+$C$6*$B11</f>
-        <v>1.0470900000000001</v>
+        <f t="shared" si="3"/>
+        <v>1.073925</v>
       </c>
       <c r="G11" s="182">
-        <f>F11/F$9-1</f>
-        <v>4.5000000000000151E-2</v>
+        <f t="shared" si="1"/>
+        <v>7.4999999999999956E-2</v>
       </c>
       <c r="H11" s="199">
-        <f t="shared" si="1"/>
-        <v>0.75000000000000255</v>
+        <f t="shared" si="4"/>
+        <v>1.2499999999999993</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B12" s="194">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="C12" s="181">
-        <f>$C$5-$C$6*$B12</f>
-        <v>0.95691000000000004</v>
+        <f t="shared" si="6"/>
+        <v>0.86413499999999999</v>
       </c>
       <c r="D12" s="182">
-        <f>C$9/C12-1</f>
-        <v>4.7120418848167533E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.1560693641618498</v>
       </c>
       <c r="E12" s="199">
-        <f t="shared" si="0"/>
-        <v>0.78534031413612559</v>
+        <f t="shared" si="2"/>
+        <v>2.6011560693641633</v>
       </c>
       <c r="F12" s="197">
-        <f>F11+$C$6*$B12</f>
-        <v>1.0921800000000002</v>
+        <f t="shared" si="3"/>
+        <v>1.1338650000000001</v>
       </c>
       <c r="G12" s="182">
-        <f>F12/F$9-1</f>
-        <v>9.000000000000008E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.13500000000000023</v>
       </c>
       <c r="H12" s="199">
-        <f t="shared" si="1"/>
-        <v>1.5000000000000013</v>
+        <f t="shared" si="4"/>
+        <v>2.250000000000004</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B13" s="194">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="C13" s="181">
-        <f>$C$5-$C$6*$B13</f>
-        <v>0.94188000000000005</v>
+        <f t="shared" si="6"/>
+        <v>0.78920999999999997</v>
       </c>
       <c r="D13" s="182">
-        <f>C$9/C13-1</f>
-        <v>6.3829787234042534E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.26582278481012667</v>
       </c>
       <c r="E13" s="199">
-        <f t="shared" si="0"/>
-        <v>1.0638297872340423</v>
+        <f t="shared" si="2"/>
+        <v>4.4303797468354444</v>
       </c>
       <c r="F13" s="197">
-        <f>F12+$C$6*$B13</f>
-        <v>1.1523000000000001</v>
+        <f t="shared" si="3"/>
+        <v>1.20879</v>
       </c>
       <c r="G13" s="182">
-        <f>F13/F$9-1</f>
-        <v>0.15000000000000013</v>
+        <f t="shared" si="1"/>
+        <v>0.20999999999999996</v>
       </c>
       <c r="H13" s="199">
-        <f t="shared" si="1"/>
-        <v>2.5000000000000022</v>
+        <f t="shared" si="4"/>
+        <v>3.4999999999999996</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B14" s="194">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
       </c>
       <c r="C14" s="181">
-        <f>$C$5-$C$6*$B14</f>
-        <v>0.92684999999999995</v>
+        <f t="shared" si="6"/>
+        <v>0.69929999999999992</v>
       </c>
       <c r="D14" s="182">
-        <f>C$9/C14-1</f>
-        <v>8.1081081081081141E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.42857142857142883</v>
       </c>
       <c r="E14" s="199">
-        <f t="shared" si="0"/>
-        <v>1.3513513513513524</v>
+        <f t="shared" si="2"/>
+        <v>7.1428571428571477</v>
       </c>
       <c r="F14" s="197">
-        <f>F13+$C$6*$B14</f>
-        <v>1.2274500000000002</v>
+        <f t="shared" si="3"/>
+        <v>1.2987</v>
       </c>
       <c r="G14" s="182">
-        <f>F14/F$9-1</f>
-        <v>0.22500000000000009</v>
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="H14" s="199">
-        <f t="shared" si="1"/>
-        <v>3.7500000000000018</v>
+        <f t="shared" si="4"/>
+        <v>5.0000000000000009</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B15" s="194">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="C15" s="181">
-        <f>$C$5-$C$6*$B15</f>
-        <v>0.91181999999999996</v>
+        <f t="shared" si="6"/>
+        <v>0.59440499999999996</v>
       </c>
       <c r="D15" s="182">
-        <f>C$9/C15-1</f>
-        <v>9.8901098901098994E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.68067226890756305</v>
       </c>
       <c r="E15" s="199">
-        <f t="shared" si="0"/>
-        <v>1.64835164835165</v>
+        <f t="shared" si="2"/>
+        <v>11.344537815126051</v>
       </c>
       <c r="F15" s="197">
-        <f>F14+$C$6*$B15</f>
-        <v>1.3176300000000001</v>
+        <f t="shared" si="3"/>
+        <v>1.4035949999999999</v>
       </c>
       <c r="G15" s="182">
-        <f>F15/F$9-1</f>
-        <v>0.31500000000000017</v>
+        <f t="shared" si="1"/>
+        <v>0.40500000000000003</v>
       </c>
       <c r="H15" s="199">
-        <f t="shared" si="1"/>
-        <v>5.2500000000000027</v>
+        <f t="shared" si="4"/>
+        <v>6.7500000000000009</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B16" s="194">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <f t="shared" si="5"/>
+        <v>8</v>
       </c>
       <c r="C16" s="181">
-        <f>$C$5-$C$6*$B16</f>
-        <v>0.89678999999999998</v>
+        <f t="shared" si="6"/>
+        <v>0.47452499999999997</v>
       </c>
       <c r="D16" s="182">
-        <f>C$9/C16-1</f>
-        <v>0.11731843575418988</v>
+        <f t="shared" si="0"/>
+        <v>1.1052631578947372</v>
       </c>
       <c r="E16" s="199">
-        <f t="shared" si="0"/>
-        <v>1.9553072625698313</v>
+        <f t="shared" si="2"/>
+        <v>18.421052631578952</v>
       </c>
       <c r="F16" s="197">
-        <f>F15+$C$6*$B16</f>
-        <v>1.4228400000000001</v>
+        <f t="shared" si="3"/>
+        <v>1.5234749999999999</v>
       </c>
       <c r="G16" s="182">
-        <f>F16/F$9-1</f>
-        <v>0.42000000000000015</v>
+        <f t="shared" si="1"/>
+        <v>0.52499999999999991</v>
       </c>
       <c r="H16" s="199">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000027</v>
+        <f t="shared" si="4"/>
+        <v>8.7499999999999982</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B17" s="194">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>9</v>
       </c>
       <c r="C17" s="181">
-        <f>$C$5-$C$6*$B17</f>
-        <v>0.88175999999999999</v>
+        <f t="shared" si="6"/>
+        <v>0.33965999999999996</v>
       </c>
       <c r="D17" s="182">
-        <f>C$9/C17-1</f>
-        <v>0.13636363636363646</v>
+        <f t="shared" si="0"/>
+        <v>1.9411764705882355</v>
       </c>
       <c r="E17" s="199">
-        <f t="shared" si="0"/>
-        <v>2.2727272727272747</v>
+        <f t="shared" si="2"/>
+        <v>32.352941176470594</v>
       </c>
       <c r="F17" s="197">
-        <f>F16+$C$6*$B17</f>
-        <v>1.54308</v>
+        <f t="shared" si="3"/>
+        <v>1.6583399999999999</v>
       </c>
       <c r="G17" s="182">
-        <f>F17/F$9-1</f>
-        <v>0.54</v>
+        <f t="shared" si="1"/>
+        <v>0.65999999999999992</v>
       </c>
       <c r="H17" s="199">
-        <f t="shared" si="1"/>
-        <v>9.0000000000000018</v>
+        <f t="shared" si="4"/>
+        <v>10.999999999999998</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B18" s="194">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
       <c r="C18" s="181">
-        <f>$C$5-$C$6*$B18</f>
-        <v>0.86673</v>
+        <f t="shared" si="6"/>
+        <v>0.18980999999999995</v>
       </c>
       <c r="D18" s="182">
-        <f>C$9/C18-1</f>
-        <v>0.1560693641618498</v>
+        <f t="shared" si="0"/>
+        <v>4.2631578947368434</v>
       </c>
       <c r="E18" s="199">
-        <f t="shared" si="0"/>
-        <v>2.6011560693641633</v>
+        <f t="shared" si="2"/>
+        <v>71.052631578947398</v>
       </c>
       <c r="F18" s="197">
-        <f>F17+$C$6*$B18</f>
-        <v>1.67835</v>
+        <f t="shared" si="3"/>
+        <v>1.80819</v>
       </c>
       <c r="G18" s="182">
-        <f>F18/F$9-1</f>
-        <v>0.67500000000000004</v>
+        <f t="shared" si="1"/>
+        <v>0.81</v>
       </c>
       <c r="H18" s="199">
-        <f t="shared" si="1"/>
-        <v>11.250000000000002</v>
+        <f t="shared" si="4"/>
+        <v>13.500000000000002</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B19" s="194">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="C19" s="181">
-        <f>$C$5-$C$6*$B19</f>
-        <v>0.85170000000000001</v>
+        <f t="shared" si="6"/>
+        <v>2.4974999999999942E-2</v>
       </c>
       <c r="D19" s="182">
-        <f>C$9/C19-1</f>
-        <v>0.17647058823529416</v>
+        <f t="shared" si="0"/>
+        <v>39.000000000000092</v>
       </c>
       <c r="E19" s="199">
-        <f t="shared" si="0"/>
-        <v>2.9411764705882359</v>
+        <f t="shared" si="2"/>
+        <v>650.00000000000159</v>
       </c>
       <c r="F19" s="197">
-        <f>F18+$C$6*$B19</f>
-        <v>1.8286500000000001</v>
+        <f t="shared" si="3"/>
+        <v>1.973025</v>
       </c>
       <c r="G19" s="182">
-        <f>F19/F$9-1</f>
-        <v>0.82500000000000018</v>
+        <f t="shared" si="1"/>
+        <v>0.97500000000000009</v>
       </c>
       <c r="H19" s="199">
-        <f t="shared" si="1"/>
-        <v>13.750000000000004</v>
+        <f t="shared" si="4"/>
+        <v>16.250000000000004</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B20" s="194">
-        <f t="shared" si="2"/>
-        <v>11</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="C20" s="181">
-        <f>$C$5-$C$6*$B20</f>
-        <v>0.83667000000000002</v>
+        <f t="shared" si="6"/>
+        <v>-0.15484500000000007</v>
       </c>
       <c r="D20" s="182">
-        <f>C$9/C20-1</f>
-        <v>0.19760479041916157</v>
+        <f t="shared" si="0"/>
+        <v>-7.4516129032258034</v>
       </c>
       <c r="E20" s="199">
-        <f t="shared" si="0"/>
-        <v>3.2934131736526928</v>
+        <f t="shared" si="2"/>
+        <v>-124.19354838709673</v>
       </c>
       <c r="F20" s="197">
-        <f>F19+$C$6*$B20</f>
-        <v>1.9939800000000001</v>
+        <f t="shared" si="3"/>
+        <v>2.1528450000000001</v>
       </c>
       <c r="G20" s="182">
-        <f>F20/F$9-1</f>
-        <v>0.99</v>
+        <f t="shared" si="1"/>
+        <v>1.1550000000000002</v>
       </c>
       <c r="H20" s="199">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
+        <f t="shared" si="4"/>
+        <v>19.250000000000004</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B21" s="194">
-        <f t="shared" si="2"/>
-        <v>12</v>
+        <f t="shared" si="5"/>
+        <v>13</v>
       </c>
       <c r="C21" s="181">
-        <f>$C$5-$C$6*$B21</f>
-        <v>0.82164000000000004</v>
+        <f t="shared" si="6"/>
+        <v>-0.34965000000000007</v>
       </c>
       <c r="D21" s="182">
-        <f>C$9/C21-1</f>
-        <v>0.21951219512195119</v>
+        <f t="shared" si="0"/>
+        <v>-3.8571428571428568</v>
       </c>
       <c r="E21" s="199">
-        <f t="shared" si="0"/>
-        <v>3.6585365853658534</v>
+        <f t="shared" si="2"/>
+        <v>-64.285714285714278</v>
       </c>
       <c r="F21" s="197">
-        <f>F20+$C$6*$B21</f>
-        <v>2.1743399999999999</v>
+        <f t="shared" si="3"/>
+        <v>2.3476500000000002</v>
       </c>
       <c r="G21" s="182">
-        <f>F21/F$9-1</f>
-        <v>1.17</v>
+        <f t="shared" si="1"/>
+        <v>1.35</v>
       </c>
       <c r="H21" s="199">
-        <f t="shared" si="1"/>
-        <v>19.5</v>
+        <f t="shared" si="4"/>
+        <v>22.500000000000004</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B22" s="194">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="C22" s="181">
-        <f>$C$5-$C$6*$B22</f>
-        <v>0.80661000000000005</v>
+        <f t="shared" si="6"/>
+        <v>-0.55944000000000005</v>
       </c>
       <c r="D22" s="182">
-        <f>C$9/C22-1</f>
-        <v>0.2422360248447204</v>
+        <f t="shared" si="0"/>
+        <v>-2.7857142857142856</v>
       </c>
       <c r="E22" s="199">
-        <f t="shared" si="0"/>
-        <v>4.0372670807453401</v>
+        <f t="shared" si="2"/>
+        <v>-46.428571428571431</v>
       </c>
       <c r="F22" s="197">
-        <f>F21+$C$6*$B22</f>
-        <v>2.3697300000000001</v>
+        <f t="shared" si="3"/>
+        <v>2.5574400000000002</v>
       </c>
       <c r="G22" s="182">
-        <f>F22/F$9-1</f>
-        <v>1.3650000000000002</v>
+        <f t="shared" si="1"/>
+        <v>1.56</v>
       </c>
       <c r="H22" s="199">
-        <f t="shared" si="1"/>
-        <v>22.750000000000004</v>
+        <f t="shared" si="4"/>
+        <v>26.000000000000004</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B23" s="194">
-        <f t="shared" si="2"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>15</v>
       </c>
       <c r="C23" s="181">
-        <f>$C$5-$C$6*$B23</f>
-        <v>0.79157999999999995</v>
+        <f t="shared" si="6"/>
+        <v>-0.78421500000000011</v>
       </c>
       <c r="D23" s="182">
-        <f>C$9/C23-1</f>
-        <v>0.26582278481012667</v>
+        <f t="shared" si="0"/>
+        <v>-2.2738853503184711</v>
       </c>
       <c r="E23" s="199">
-        <f t="shared" si="0"/>
-        <v>4.4303797468354444</v>
+        <f t="shared" si="2"/>
+        <v>-37.898089171974519</v>
       </c>
       <c r="F23" s="197">
-        <f>F22+$C$6*$B23</f>
-        <v>2.5801500000000002</v>
+        <f t="shared" si="3"/>
+        <v>2.7822150000000003</v>
       </c>
       <c r="G23" s="182">
-        <f>F23/F$9-1</f>
-        <v>1.5750000000000002</v>
+        <f t="shared" si="1"/>
+        <v>1.7850000000000001</v>
       </c>
       <c r="H23" s="199">
-        <f t="shared" si="1"/>
-        <v>26.250000000000004</v>
+        <f t="shared" si="4"/>
+        <v>29.750000000000004</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B24" s="194">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="C24" s="181">
-        <f>$C$5-$C$6*$B24</f>
-        <v>0.77654999999999996</v>
+        <f t="shared" si="6"/>
+        <v>-1.0239750000000001</v>
       </c>
       <c r="D24" s="182">
-        <f>C$9/C24-1</f>
-        <v>0.29032258064516125</v>
+        <f t="shared" si="0"/>
+        <v>-1.975609756097561</v>
       </c>
       <c r="E24" s="199">
-        <f t="shared" si="0"/>
-        <v>4.8387096774193541</v>
+        <f t="shared" si="2"/>
+        <v>-32.926829268292686</v>
       </c>
       <c r="F24" s="197">
-        <f>F23+$C$6*$B24</f>
-        <v>2.8056000000000001</v>
+        <f t="shared" si="3"/>
+        <v>3.0219750000000003</v>
       </c>
       <c r="G24" s="182">
-        <f>F24/F$9-1</f>
-        <v>1.8000000000000003</v>
+        <f t="shared" si="1"/>
+        <v>2.0250000000000004</v>
       </c>
       <c r="H24" s="199">
-        <f t="shared" si="1"/>
-        <v>30.000000000000007</v>
+        <f t="shared" si="4"/>
+        <v>33.750000000000007</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B25" s="194">
-        <f t="shared" si="2"/>
-        <v>16</v>
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
       <c r="C25" s="181">
-        <f>$C$5-$C$6*$B25</f>
-        <v>0.76151999999999997</v>
+        <f t="shared" si="6"/>
+        <v>-1.2787200000000001</v>
       </c>
       <c r="D25" s="182">
-        <f>C$9/C25-1</f>
-        <v>0.31578947368421062</v>
+        <f t="shared" si="0"/>
+        <v>-1.78125</v>
       </c>
       <c r="E25" s="199">
-        <f t="shared" si="0"/>
-        <v>5.2631578947368443</v>
+        <f t="shared" si="2"/>
+        <v>-29.6875</v>
       </c>
       <c r="F25" s="197">
-        <f>F24+$C$6*$B25</f>
-        <v>3.0460799999999999</v>
+        <f t="shared" si="3"/>
+        <v>3.2767200000000001</v>
       </c>
       <c r="G25" s="182">
-        <f>F25/F$9-1</f>
-        <v>2.04</v>
+        <f t="shared" si="1"/>
+        <v>2.2800000000000002</v>
       </c>
       <c r="H25" s="199">
-        <f t="shared" si="1"/>
-        <v>34</v>
+        <f t="shared" si="4"/>
+        <v>38.000000000000007</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B26" s="194">
-        <f t="shared" si="2"/>
-        <v>17</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="C26" s="181">
-        <f>$C$5-$C$6*$B26</f>
-        <v>0.74648999999999999</v>
+        <f t="shared" si="6"/>
+        <v>-1.5484500000000001</v>
       </c>
       <c r="D26" s="182">
-        <f>C$9/C26-1</f>
-        <v>0.34228187919463093</v>
+        <f t="shared" si="0"/>
+        <v>-1.6451612903225805</v>
       </c>
       <c r="E26" s="199">
-        <f t="shared" si="0"/>
-        <v>5.7046979865771821</v>
+        <f t="shared" si="2"/>
+        <v>-27.419354838709676</v>
       </c>
       <c r="F26" s="197">
-        <f>F25+$C$6*$B26</f>
-        <v>3.30159</v>
+        <f t="shared" si="3"/>
+        <v>3.5464500000000001</v>
       </c>
       <c r="G26" s="182">
-        <f>F26/F$9-1</f>
-        <v>2.2949999999999999</v>
+        <f t="shared" si="1"/>
+        <v>2.5500000000000003</v>
       </c>
       <c r="H26" s="199">
-        <f t="shared" si="1"/>
-        <v>38.25</v>
+        <f t="shared" si="4"/>
+        <v>42.500000000000007</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B27" s="194">
-        <f t="shared" si="2"/>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>19</v>
       </c>
       <c r="C27" s="181">
-        <f>$C$5-$C$6*$B27</f>
-        <v>0.73146</v>
+        <f t="shared" si="6"/>
+        <v>-1.8331650000000002</v>
       </c>
       <c r="D27" s="182">
-        <f>C$9/C27-1</f>
-        <v>0.36986301369863006</v>
+        <f t="shared" si="0"/>
+        <v>-1.5449591280653951</v>
       </c>
       <c r="E27" s="199">
-        <f t="shared" si="0"/>
-        <v>6.1643835616438345</v>
+        <f t="shared" si="2"/>
+        <v>-25.74931880108992</v>
       </c>
       <c r="F27" s="197">
-        <f>F26+$C$6*$B27</f>
-        <v>3.57213</v>
+        <f t="shared" si="3"/>
+        <v>3.8311649999999999</v>
       </c>
       <c r="G27" s="182">
-        <f>F27/F$9-1</f>
-        <v>2.5649999999999999</v>
+        <f t="shared" si="1"/>
+        <v>2.835</v>
       </c>
       <c r="H27" s="199">
-        <f t="shared" si="1"/>
-        <v>42.75</v>
+        <f t="shared" si="4"/>
+        <v>47.25</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B28" s="195">
-        <f t="shared" si="2"/>
-        <v>19</v>
+        <f t="shared" si="5"/>
+        <v>20</v>
       </c>
       <c r="C28" s="186">
-        <f>$C$5-$C$6*$B28</f>
-        <v>0.71643000000000001</v>
+        <f t="shared" si="6"/>
+        <v>-2.1328650000000002</v>
       </c>
       <c r="D28" s="187">
-        <f>C$9/C28-1</f>
-        <v>0.39860139860139854</v>
+        <f t="shared" si="0"/>
+        <v>-1.4683840749414521</v>
       </c>
       <c r="E28" s="200">
-        <f t="shared" si="0"/>
-        <v>6.6433566433566424</v>
+        <f t="shared" si="2"/>
+        <v>-24.473067915690869</v>
       </c>
       <c r="F28" s="198">
-        <f>F27+$C$6*$B28</f>
-        <v>3.8576999999999999</v>
+        <f t="shared" si="3"/>
+        <v>4.130865</v>
       </c>
       <c r="G28" s="187">
-        <f>F28/F$9-1</f>
-        <v>2.85</v>
+        <f t="shared" si="1"/>
+        <v>3.1349999999999998</v>
       </c>
       <c r="H28" s="200">
-        <f t="shared" si="1"/>
-        <v>47.5</v>
+        <f t="shared" si="4"/>
+        <v>52.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>